<commit_message>
Added confirmation-page and implemented logout-function (not tested yet)
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Jonas\Programmierung\Ionic\WildShop\WNodeJS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\Entwicklung\WildShop\WNodeJS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB3779A-2BA6-4C0F-B5A2-5339925475C6}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07164FB9-0E41-4581-A6CF-1EBC17136519}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12312" xr2:uid="{659A3680-8E12-4613-AC7A-D48333959E04}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315" xr2:uid="{659A3680-8E12-4613-AC7A-D48333959E04}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
   <si>
     <t>TODO</t>
   </si>
@@ -61,13 +61,22 @@
   </si>
   <si>
     <t>Jonas</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>E-Mail versenden nach Bestellung</t>
+  </si>
+  <si>
+    <t>Logout</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,8 +91,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -93,6 +109,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -109,9 +131,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Schlecht" xfId="1" builtinId="27"/>
@@ -455,18 +478,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D9FE81-AB7B-4C47-91AF-D3A27946C115}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="69.109375" customWidth="1"/>
+    <col min="1" max="1" width="69.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -477,18 +500,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>10</v>
+      <c r="B2" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -499,7 +522,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -507,7 +530,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -515,7 +538,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -526,7 +549,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -534,12 +557,34 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Re-wite of addOrder (not finished)
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\Entwicklung\WildShop\WNodeJS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Jonas\Programmierung\Ionic\WildShop\WNodeJS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07164FB9-0E41-4581-A6CF-1EBC17136519}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D6E98D-BA86-421B-9E30-CE80A94D9C6E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315" xr2:uid="{659A3680-8E12-4613-AC7A-D48333959E04}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12312" xr2:uid="{659A3680-8E12-4613-AC7A-D48333959E04}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
   <si>
     <t>TODO</t>
   </si>
@@ -70,13 +70,25 @@
   </si>
   <si>
     <t>Logout</t>
+  </si>
+  <si>
+    <t>in Arbeit</t>
+  </si>
+  <si>
+    <t>Hinweis</t>
+  </si>
+  <si>
+    <t>Cron-Job</t>
+  </si>
+  <si>
+    <t>addOrder umschreiben</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,8 +110,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -117,6 +144,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -127,16 +159,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Schlecht" xfId="1" builtinId="27"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -478,29 +514,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D9FE81-AB7B-4C47-91AF-D3A27946C115}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="69.140625" customWidth="1"/>
+    <col min="1" max="1" width="69.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -511,7 +550,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -522,7 +561,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -530,7 +569,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -538,7 +577,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -548,8 +587,11 @@
       <c r="C6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -557,7 +599,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -565,7 +607,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -576,14 +618,25 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>10</v>
+      <c r="B10" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="C10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Logout basically working, just on Home -> implementation is the same on every page
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Jonas\Programmierung\Ionic\WildShop\WNodeJS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D6E98D-BA86-421B-9E30-CE80A94D9C6E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{700EE4AA-4782-4112-9F9B-EE5A6F6F59E1}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12312" xr2:uid="{659A3680-8E12-4613-AC7A-D48333959E04}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
   <si>
     <t>TODO</t>
   </si>
@@ -82,6 +82,15 @@
   </si>
   <si>
     <t>addOrder umschreiben</t>
+  </si>
+  <si>
+    <t>Jesse, Jonas</t>
+  </si>
+  <si>
+    <t>Jesse</t>
+  </si>
+  <si>
+    <t>Login zurückgehen in Login-Page verhindern</t>
   </si>
 </sst>
 </file>
@@ -514,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D9FE81-AB7B-4C47-91AF-D3A27946C115}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -568,6 +577,9 @@
       <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -576,6 +588,9 @@
       <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -598,6 +613,9 @@
       <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -606,6 +624,9 @@
       <c r="B8" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -633,11 +654,16 @@
       <c r="A11" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>15</v>
+      <c r="B11" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="C11" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
style is a bit more fancy, mailController is new and has basic functionality but doesn't send mails yet
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Jonas\Programmierung\Ionic\WildShop\WNodeJS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\Entwicklung\WildShop\WNodeJS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BCCC509-E7B2-4080-AB5C-B6B437B663DF}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61776951-2F80-40CC-8CED-837E1E348FC0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12312" xr2:uid="{659A3680-8E12-4613-AC7A-D48333959E04}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315" xr2:uid="{659A3680-8E12-4613-AC7A-D48333959E04}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
   <si>
     <t>TODO</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Seite, die Angebot verwaltet. Soll auch Übersicht über alle Bestellungen zeigen</t>
   </si>
   <si>
-    <t>Einteilung der Produkte in Kategorien</t>
-  </si>
-  <si>
     <t>Suche</t>
   </si>
   <si>
@@ -91,6 +88,15 @@
   </si>
   <si>
     <t>Login zurückgehen in Login-Page verhindern</t>
+  </si>
+  <si>
+    <t>Logging-System</t>
+  </si>
+  <si>
+    <t>Einteilung der Produkte in Kategorien -&gt; neue Spalte in DB-Tabelle</t>
+  </si>
+  <si>
+    <t>Bilder neben Produkten anzeigen -&gt; neue Spalte in DB-Tabelle, die Pfad zum Bild anzeigt</t>
   </si>
 </sst>
 </file>
@@ -523,18 +529,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D9FE81-AB7B-4C47-91AF-D3A27946C115}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="69.109375" customWidth="1"/>
+    <col min="1" max="1" width="69.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -545,125 +551,150 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="1" t="s">
+      <c r="C11" t="s">
         <v>10</v>
       </c>
-      <c r="C7" t="s">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="B12" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C14" t="s">
         <v>10</v>
-      </c>
-      <c r="C8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mails will be sent now after order
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\Entwicklung\WildShop\WNodeJS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61776951-2F80-40CC-8CED-837E1E348FC0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79032B5D-9FFD-46D1-A30C-836B2FEE76B9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315" xr2:uid="{659A3680-8E12-4613-AC7A-D48333959E04}"/>
   </bookViews>
@@ -532,7 +532,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,8 +638,8 @@
       <c r="A9" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>9</v>
+      <c r="B9" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Added new order-system. Now every order just exists with one hash in the database.
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\Entwicklung\WildShop\WNodeJS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79032B5D-9FFD-46D1-A30C-836B2FEE76B9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECCC328E-0F07-4506-AD21-5F3C94B90266}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315" xr2:uid="{659A3680-8E12-4613-AC7A-D48333959E04}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
   <si>
     <t>TODO</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>Bilder neben Produkten anzeigen -&gt; neue Spalte in DB-Tabelle, die Pfad zum Bild anzeigt</t>
+  </si>
+  <si>
+    <t>Generierung eines Order-ID-Hashes, der als eindeutige Order-ID genutzt wird -&gt; darauf aufbauend Verhindern der Trennung von Orders, weil bei jedem Produkt Bestand geprüft wird</t>
   </si>
 </sst>
 </file>
@@ -529,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D9FE81-AB7B-4C47-91AF-D3A27946C115}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,8 +641,8 @@
       <c r="A9" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>14</v>
+      <c r="B9" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
@@ -649,8 +652,8 @@
       <c r="A10" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>14</v>
+      <c r="B10" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
@@ -694,6 +697,17 @@
         <v>9</v>
       </c>
       <c r="C14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Products can now be removed of the cart. Blind coded parts of the logger are includede, probably buggy.
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\Entwicklung\WildShop\WNodeJS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECCC328E-0F07-4506-AD21-5F3C94B90266}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{304B719D-15D6-4705-88AB-8290CA46FF14}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315" xr2:uid="{659A3680-8E12-4613-AC7A-D48333959E04}"/>
   </bookViews>
@@ -535,7 +535,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,11 +594,11 @@
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
+      <c r="B5" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added authorization-system after registration. DB must be reinitialized. Some changes concerning the constants...
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\Entwicklung\WildShop\WNodeJS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Jonas\Programmierung\Ionic\WildShop\WNodeJS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{304B719D-15D6-4705-88AB-8290CA46FF14}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F85210A-7BA4-4011-A0D6-CC40452938A9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315" xr2:uid="{659A3680-8E12-4613-AC7A-D48333959E04}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12312" xr2:uid="{659A3680-8E12-4613-AC7A-D48333959E04}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -535,15 +535,15 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="69.140625" customWidth="1"/>
+    <col min="1" max="1" width="69.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -557,7 +557,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -568,7 +568,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -579,7 +579,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -590,18 +590,18 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>14</v>
+      <c r="B5" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="C5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -615,7 +615,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -626,7 +626,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -637,7 +637,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -648,7 +648,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -659,7 +659,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -670,7 +670,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -678,7 +678,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -689,7 +689,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -700,7 +700,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
Logger added, works synchrouniously...check if it's possible to implement asynchrouniously (Threads or async functions?)
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Jonas\Programmierung\Ionic\WildShop\WNodeJS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\Entwicklung\WildShop\WNodeJS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F85210A-7BA4-4011-A0D6-CC40452938A9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F28E8E2-4D1E-4AA5-AF24-E38E395F9B29}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12312" xr2:uid="{659A3680-8E12-4613-AC7A-D48333959E04}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315" xr2:uid="{659A3680-8E12-4613-AC7A-D48333959E04}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="25">
   <si>
     <t>TODO</t>
   </si>
@@ -69,9 +69,6 @@
     <t>Logout</t>
   </si>
   <si>
-    <t>in Arbeit</t>
-  </si>
-  <si>
     <t>Hinweis</t>
   </si>
   <si>
@@ -100,13 +97,16 @@
   </si>
   <si>
     <t>Generierung eines Order-ID-Hashes, der als eindeutige Order-ID genutzt wird -&gt; darauf aufbauend Verhindern der Trennung von Orders, weil bei jedem Produkt Bestand geprüft wird</t>
+  </si>
+  <si>
+    <t>Konstanten in JSON-File</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,13 +129,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,7 +137,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -162,11 +155,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -177,20 +165,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
+  <cellStyles count="2">
     <cellStyle name="Schlecht" xfId="1" builtinId="27"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -532,32 +517,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D9FE81-AB7B-4C47-91AF-D3A27946C115}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="69.109375" customWidth="1"/>
+    <col min="1" max="1" width="69.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D1" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -568,7 +553,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -579,7 +564,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -587,10 +572,10 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -598,10 +583,10 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -612,21 +597,21 @@
         <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -634,10 +619,10 @@
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -648,7 +633,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -659,9 +644,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>11</v>
@@ -670,28 +655,28 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>14</v>
+      <c r="B13" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="C13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>9</v>
@@ -700,14 +685,25 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="B16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added password-changing-function (blind coded and not tested)
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Jonas\Programmierung\Ionic\WildShop\WNodeJS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F85210A-7BA4-4011-A0D6-CC40452938A9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A36C734-8A4F-47F6-A836-1B288A6B5507}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12312" xr2:uid="{659A3680-8E12-4613-AC7A-D48333959E04}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="29">
   <si>
     <t>TODO</t>
   </si>
@@ -100,6 +100,18 @@
   </si>
   <si>
     <t>Generierung eines Order-ID-Hashes, der als eindeutige Order-ID genutzt wird -&gt; darauf aufbauend Verhindern der Trennung von Orders, weil bei jedem Produkt Bestand geprüft wird</t>
+  </si>
+  <si>
+    <t>optional</t>
+  </si>
+  <si>
+    <t>User löschen</t>
+  </si>
+  <si>
+    <t>Joans</t>
+  </si>
+  <si>
+    <t>Passwort ändern/vergessen</t>
   </si>
 </sst>
 </file>
@@ -144,7 +156,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -167,6 +179,12 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -182,12 +200,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
@@ -532,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D9FE81-AB7B-4C47-91AF-D3A27946C115}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -619,8 +638,8 @@
       <c r="A7" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>9</v>
+      <c r="B7" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
@@ -630,8 +649,8 @@
       <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>9</v>
+      <c r="B8" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="C8" t="s">
         <v>19</v>
@@ -682,8 +701,8 @@
       <c r="A13" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>14</v>
+      <c r="B13" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="C13" t="s">
         <v>10</v>
@@ -711,7 +730,27 @@
         <v>10</v>
       </c>
     </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
forgot password-function is now tested and aviable...some error-handling is still missing.
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Jonas\Programmierung\Ionic\WildShop\WNodeJS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A36C734-8A4F-47F6-A836-1B288A6B5507}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54BA7D23-1829-4937-8274-4C7791D6D425}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12312" xr2:uid="{659A3680-8E12-4613-AC7A-D48333959E04}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
   <si>
     <t>TODO</t>
   </si>
@@ -67,9 +67,6 @@
   </si>
   <si>
     <t>Logout</t>
-  </si>
-  <si>
-    <t>in Arbeit</t>
   </si>
   <si>
     <t>Hinweis</t>
@@ -118,7 +115,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,13 +138,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,7 +146,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -176,11 +166,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -195,21 +180,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
+  <cellStyles count="2">
     <cellStyle name="Schlecht" xfId="1" builtinId="27"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -554,7 +536,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -563,17 +545,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>15</v>
+      <c r="D1" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -606,7 +588,7 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -617,7 +599,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -631,29 +613,29 @@
         <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>25</v>
+        <v>21</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>25</v>
+      <c r="B8" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -680,7 +662,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>11</v>
@@ -691,7 +673,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>11</v>
@@ -699,7 +681,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>11</v>
@@ -710,7 +692,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>9</v>
@@ -721,7 +703,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>11</v>
@@ -732,21 +714,21 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s">
         <v>26</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>14</v>
+        <v>27</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Shopping-Cart will be saved now with logout
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Jonas\Programmierung\Ionic\WildShop\WNodeJS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54BA7D23-1829-4937-8274-4C7791D6D425}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37DED5E8-A6D5-49EE-91A5-3F49322A1AF9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12312" xr2:uid="{659A3680-8E12-4613-AC7A-D48333959E04}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="30">
   <si>
     <t>TODO</t>
   </si>
@@ -109,6 +109,12 @@
   </si>
   <si>
     <t>Passwort ändern/vergessen</t>
+  </si>
+  <si>
+    <t>Einkaufswagen in DB speichern</t>
+  </si>
+  <si>
+    <t>Logs überall einfügen, allgemeine Fehlerprevention/Abfangen der Fehler</t>
   </si>
 </sst>
 </file>
@@ -533,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D9FE81-AB7B-4C47-91AF-D3A27946C115}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -694,8 +700,8 @@
       <c r="A14" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>9</v>
+      <c r="B14" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="C14" t="s">
         <v>10</v>
@@ -729,6 +735,22 @@
       </c>
       <c r="B17" s="2" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Shopping cart improved, styling
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Jonas\Programmierung\Ionic\WildShop\WNodeJS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E9DFAA2-FB92-462D-8079-CEB123A052B6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCBC6F8A-810F-40CB-B699-8F23A5EE9C42}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12312" xr2:uid="{659A3680-8E12-4613-AC7A-D48333959E04}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="34">
   <si>
     <t>TODO</t>
   </si>
@@ -121,6 +121,12 @@
   </si>
   <si>
     <t>Funktionen wie logout() und goToConfirmation in Provider packen</t>
+  </si>
+  <si>
+    <t>E-Mail -&gt; Texte überarbeiten (eventuell mit HTML was machen?)</t>
+  </si>
+  <si>
+    <t>Tests</t>
   </si>
 </sst>
 </file>
@@ -545,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D9FE81-AB7B-4C47-91AF-D3A27946C115}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -735,7 +741,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -743,7 +749,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -751,27 +757,38 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>28</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B20" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added test-cases to Excel-document
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Jonas\Programmierung\Ionic\WildShop\WNodeJS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\Entwicklung\WildShop\WNodeJS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCBC6F8A-810F-40CB-B699-8F23A5EE9C42}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{788A56EE-A576-4C53-A415-36BC40A61631}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12312" xr2:uid="{659A3680-8E12-4613-AC7A-D48333959E04}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315" xr2:uid="{659A3680-8E12-4613-AC7A-D48333959E04}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="TODO" sheetId="1" r:id="rId1"/>
+    <sheet name="Testfälle" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="56">
   <si>
     <t>TODO</t>
   </si>
@@ -126,14 +127,80 @@
     <t>E-Mail -&gt; Texte überarbeiten (eventuell mit HTML was machen?)</t>
   </si>
   <si>
-    <t>Tests</t>
+    <t xml:space="preserve">Testfall </t>
+  </si>
+  <si>
+    <t>Ergebnis</t>
+  </si>
+  <si>
+    <t>Login durchführen</t>
+  </si>
+  <si>
+    <t>Registrierung vollständig durchführen</t>
+  </si>
+  <si>
+    <t>Registrierung mit freien Feldern versuchen</t>
+  </si>
+  <si>
+    <t>Passwort vergessen vollständig undangemeldet durchführen</t>
+  </si>
+  <si>
+    <t>Passwort vergessen unvollständig unangemeldet durchführen</t>
+  </si>
+  <si>
+    <t>Passwort vergessen vollständig angemeldet durchführen</t>
+  </si>
+  <si>
+    <t>Passwort vergessen unvollständig angemeldet durchfüren</t>
+  </si>
+  <si>
+    <t>Account löschen</t>
+  </si>
+  <si>
+    <t>Bestellungsprozess einmal vollständig mit 1 Produkt durchführen</t>
+  </si>
+  <si>
+    <t>Bestellungsprozess vollständig mit mehreren Produkten durchführen</t>
+  </si>
+  <si>
+    <t>Bestellungsprozess in der Mitte abbrechen (durch Logout)</t>
+  </si>
+  <si>
+    <t>Bestellungsprozess abbrechen mit Schließen des Fensters</t>
+  </si>
+  <si>
+    <t>Produkte aus Warenkorb entfernen</t>
+  </si>
+  <si>
+    <t>Produkte zu Warenkorb hinzufügen</t>
+  </si>
+  <si>
+    <t>Produkt mit Kommentar in Warenkorb hinzufügen und bestellen</t>
+  </si>
+  <si>
+    <t>Produkt mehrmals mit Kommentar in Warenkorb hinzufügen und bestellen</t>
+  </si>
+  <si>
+    <t>Produkt ohne Kommentar in Warenkorb hinzufügen und bestellen</t>
+  </si>
+  <si>
+    <t>Produkt ohne Kommentar mehrmals in Warenkorb hinzufügen und bestellen</t>
+  </si>
+  <si>
+    <t>Nach Registrierung versuchen zu bestellen, ohne Account verifiziert zu haben</t>
+  </si>
+  <si>
+    <t>Verfizierung des Accounts durchführen</t>
+  </si>
+  <si>
+    <t>Einfügen bei Tests</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,8 +230,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -188,6 +270,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -202,12 +290,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Schlecht" xfId="1" builtinId="27"/>
@@ -553,16 +643,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D9FE81-AB7B-4C47-91AF-D3A27946C115}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="69.109375" customWidth="1"/>
+    <col min="1" max="1" width="69.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -576,7 +666,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -587,7 +677,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -598,7 +688,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -609,7 +699,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -620,7 +710,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -634,7 +724,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -645,7 +735,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -656,7 +746,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -667,7 +757,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -678,7 +768,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -689,7 +779,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -697,7 +787,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -708,7 +798,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -719,7 +809,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -730,7 +820,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -741,7 +831,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -749,7 +839,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -757,7 +847,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>28</v>
       </c>
@@ -765,10 +855,10 @@
         <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -776,7 +866,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -784,7 +874,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -796,4 +886,131 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{398800B4-0215-4759-8FBC-1CB8B7366E83}">
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="82.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Price is shown in confirmation-mails now.
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\Entwicklung\WildShop\WNodeJS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Jonas\Programmierung\Ionic\WildShop\WNodeJS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{788A56EE-A576-4C53-A415-36BC40A61631}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C84106-060E-46B9-9E82-E470B2DD9D76}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315" xr2:uid="{659A3680-8E12-4613-AC7A-D48333959E04}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12312" xr2:uid="{659A3680-8E12-4613-AC7A-D48333959E04}"/>
   </bookViews>
   <sheets>
     <sheet name="TODO" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="58">
   <si>
     <t>TODO</t>
   </si>
@@ -194,6 +194,12 @@
   </si>
   <si>
     <t>Einfügen bei Tests</t>
+  </si>
+  <si>
+    <t>verschoben</t>
+  </si>
+  <si>
+    <t>Preis in Email: Preis an sendMail in mailController übergeben, in mailController eigene price-Hashlist anlegen, die nach userID sortiert ist. Beim Senden der Mail den Preis rausholen und Eintrag löschen. Preis wir din requestController berechnet</t>
   </si>
 </sst>
 </file>
@@ -246,7 +252,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -276,6 +282,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -290,7 +302,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
@@ -298,6 +310,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Schlecht" xfId="1" builtinId="27"/>
@@ -641,18 +654,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D9FE81-AB7B-4C47-91AF-D3A27946C115}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="69.140625" customWidth="1"/>
+    <col min="1" max="1" width="69.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -666,7 +679,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -677,7 +690,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -688,7 +701,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -699,7 +712,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -710,7 +723,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -724,7 +737,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -735,7 +748,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -746,7 +759,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -757,7 +770,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -768,7 +781,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -779,7 +792,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -787,7 +800,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -798,18 +811,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>9</v>
+      <c r="B14" s="7" t="s">
+        <v>56</v>
       </c>
       <c r="C14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -820,7 +833,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -831,7 +844,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -839,7 +852,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -847,7 +860,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>28</v>
       </c>
@@ -858,7 +871,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -866,7 +879,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -874,12 +887,20 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>32</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -896,12 +917,12 @@
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="82.85546875" customWidth="1"/>
+    <col min="1" max="1" width="82.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>33</v>
       </c>
@@ -909,102 +930,102 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>54</v>
       </c>

</xml_diff>

<commit_message>
Fixed change password-function, added style to last page and added definition of the CMS to Anforderungen.docx
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Jonas\Programmierung\Ionic\WildShop\WNodeJS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C84106-060E-46B9-9E82-E470B2DD9D76}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B907FD2-243B-4D42-AE66-B0D00FC097AA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12312" xr2:uid="{659A3680-8E12-4613-AC7A-D48333959E04}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="64">
   <si>
     <t>TODO</t>
   </si>
@@ -130,9 +130,6 @@
     <t xml:space="preserve">Testfall </t>
   </si>
   <si>
-    <t>Ergebnis</t>
-  </si>
-  <si>
     <t>Login durchführen</t>
   </si>
   <si>
@@ -200,6 +197,27 @@
   </si>
   <si>
     <t>Preis in Email: Preis an sendMail in mailController übergeben, in mailController eigene price-Hashlist anlegen, die nach userID sortiert ist. Beim Senden der Mail den Preis rausholen und Eintrag löschen. Preis wir din requestController berechnet</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Ergebnis Testlauf 1</t>
+  </si>
+  <si>
+    <t>Ergebnis Testlauf 2</t>
+  </si>
+  <si>
+    <t>OK, zweiter Test ratsam</t>
+  </si>
+  <si>
+    <t>URLs bei Bestätigung ändern</t>
+  </si>
+  <si>
+    <t>bei Release</t>
+  </si>
+  <si>
+    <t>Strings etc. in Konstanten umwandeln</t>
   </si>
 </sst>
 </file>
@@ -252,7 +270,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -288,6 +306,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -302,7 +332,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
@@ -311,6 +341,9 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Schlecht" xfId="1" builtinId="27"/>
@@ -654,15 +687,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D9FE81-AB7B-4C47-91AF-D3A27946C115}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="69.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.77734375" customWidth="1"/>
+    <col min="3" max="3" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -816,7 +851,7 @@
         <v>30</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C14" t="s">
         <v>10</v>
@@ -868,7 +903,7 @@
         <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -897,10 +932,26 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -911,123 +962,146 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{398800B4-0215-4759-8FBC-1CB8B7366E83}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="82.88671875" customWidth="1"/>
+    <col min="2" max="2" width="44.109375" customWidth="1"/>
+    <col min="3" max="3" width="41.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>33</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B2" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="B4" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="B5" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="B6" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="B7" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="B8" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Login works, registration works in CMS.
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Jonas\Programmierung\Ionic\WildShop\WNodeJS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B907FD2-243B-4D42-AE66-B0D00FC097AA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0952D12B-52D9-4BF9-96B4-A9EC373B5206}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12312" xr2:uid="{659A3680-8E12-4613-AC7A-D48333959E04}"/>
   </bookViews>
   <sheets>
     <sheet name="TODO" sheetId="1" r:id="rId1"/>
-    <sheet name="Testfälle" sheetId="2" r:id="rId2"/>
+    <sheet name="TODO CMS" sheetId="3" r:id="rId2"/>
+    <sheet name="Testfälle" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -961,6 +962,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B04E74DD-7DA5-47AC-8294-8183086F3F5E}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{398800B4-0215-4759-8FBC-1CB8B7366E83}">
   <dimension ref="A1:C21"/>
   <sheetViews>

</xml_diff>

<commit_message>
Products are shown now on the CMS-homepage. Deleting and adding products is blind coded in backend, not tested yet.
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Jonas\Programmierung\Ionic\WildShop\WNodeJS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0952D12B-52D9-4BF9-96B4-A9EC373B5206}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55A7E639-6E58-44D2-90A5-6FEFD3592E3A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12312" xr2:uid="{659A3680-8E12-4613-AC7A-D48333959E04}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12312" activeTab="1" xr2:uid="{659A3680-8E12-4613-AC7A-D48333959E04}"/>
   </bookViews>
   <sheets>
     <sheet name="TODO" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="71">
   <si>
     <t>TODO</t>
   </si>
@@ -219,6 +219,27 @@
   </si>
   <si>
     <t>Strings etc. in Konstanten umwandeln</t>
+  </si>
+  <si>
+    <t>Löschen von Bestellungen</t>
+  </si>
+  <si>
+    <t>Löschen von Usern</t>
+  </si>
+  <si>
+    <t>Produkte löschen</t>
+  </si>
+  <si>
+    <t>Produkte hinzufügen</t>
+  </si>
+  <si>
+    <t>Verifikation von neuen Admin-Usern</t>
+  </si>
+  <si>
+    <t>Passwort ändern</t>
+  </si>
+  <si>
+    <t>Anzeigen aller Produkte</t>
   </si>
 </sst>
 </file>
@@ -690,8 +711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D9FE81-AB7B-4C47-91AF-D3A27946C115}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -963,12 +984,120 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B04E74DD-7DA5-47AC-8294-8183086F3F5E}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="36.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -978,7 +1107,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1011,6 +1140,9 @@
       <c r="A3" t="s">
         <v>35</v>
       </c>
+      <c r="B3" s="8" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">

</xml_diff>

<commit_message>
Added some pages and functionality concerning order-list and order-details.
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Jonas\Programmierung\Ionic\WildShop\WNodeJS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55A7E639-6E58-44D2-90A5-6FEFD3592E3A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65383561-53AA-41C6-BF64-EEA63E69DBCC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12312" activeTab="1" xr2:uid="{659A3680-8E12-4613-AC7A-D48333959E04}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="72">
   <si>
     <t>TODO</t>
   </si>
@@ -240,6 +240,9 @@
   </si>
   <si>
     <t>Anzeigen aller Produkte</t>
+  </si>
+  <si>
+    <t>Bei Veränderung des Amounts von 0 auf &gt;0 -&gt; Mail an alle Vorbesteller senden, dass Produkt jetzt verfügbar und bestellt ist</t>
   </si>
 </sst>
 </file>
@@ -984,10 +987,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B04E74DD-7DA5-47AC-8294-8183086F3F5E}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1094,6 +1097,17 @@
         <v>11</v>
       </c>
       <c r="C9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Bugfixes. Added some standard-functionality.
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Jonas\Programmierung\Ionic\WildShop\WNodeJS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\Entwicklung\WildShop\WNodeJS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65383561-53AA-41C6-BF64-EEA63E69DBCC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B18E427C-4338-41BD-8619-EC25CCE86BD9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12312" activeTab="1" xr2:uid="{659A3680-8E12-4613-AC7A-D48333959E04}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315" activeTab="1" xr2:uid="{659A3680-8E12-4613-AC7A-D48333959E04}"/>
   </bookViews>
   <sheets>
     <sheet name="TODO" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="73">
   <si>
     <t>TODO</t>
   </si>
@@ -243,6 +243,9 @@
   </si>
   <si>
     <t>Bei Veränderung des Amounts von 0 auf &gt;0 -&gt; Mail an alle Vorbesteller senden, dass Produkt jetzt verfügbar und bestellt ist</t>
+  </si>
+  <si>
+    <t>Order anhand orderID suchen können</t>
   </si>
 </sst>
 </file>
@@ -718,14 +721,14 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="69.109375" customWidth="1"/>
-    <col min="2" max="2" width="17.77734375" customWidth="1"/>
-    <col min="3" max="3" width="15.77734375" customWidth="1"/>
+    <col min="1" max="1" width="69.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -739,7 +742,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -750,7 +753,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -761,7 +764,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -772,7 +775,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -783,7 +786,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -797,7 +800,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -808,7 +811,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -819,7 +822,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -830,7 +833,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -841,7 +844,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -852,7 +855,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -860,7 +863,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -871,7 +874,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -882,7 +885,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -893,7 +896,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -904,7 +907,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -912,7 +915,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -920,7 +923,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>28</v>
       </c>
@@ -931,7 +934,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -939,7 +942,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -947,7 +950,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -955,7 +958,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>56</v>
       </c>
@@ -963,7 +966,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>61</v>
       </c>
@@ -971,7 +974,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>63</v>
       </c>
@@ -987,18 +990,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B04E74DD-7DA5-47AC-8294-8183086F3F5E}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.88671875" customWidth="1"/>
+    <col min="1" max="1" width="36.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1012,7 +1015,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>64</v>
       </c>
@@ -1023,18 +1026,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>65</v>
       </c>
@@ -1045,7 +1048,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>66</v>
       </c>
@@ -1056,7 +1059,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>67</v>
       </c>
@@ -1067,7 +1070,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>68</v>
       </c>
@@ -1078,7 +1081,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>69</v>
       </c>
@@ -1089,7 +1092,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>70</v>
       </c>
@@ -1100,7 +1103,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>71</v>
       </c>
@@ -1108,6 +1111,17 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1124,14 +1138,14 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="82.88671875" customWidth="1"/>
-    <col min="2" max="2" width="44.109375" customWidth="1"/>
-    <col min="3" max="3" width="41.77734375" customWidth="1"/>
+    <col min="1" max="1" width="82.85546875" customWidth="1"/>
+    <col min="2" max="2" width="44.140625" customWidth="1"/>
+    <col min="3" max="3" width="41.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>33</v>
       </c>
@@ -1142,7 +1156,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -1150,7 +1164,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -1158,7 +1172,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -1166,7 +1180,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -1174,7 +1188,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -1182,7 +1196,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -1190,7 +1204,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -1198,67 +1212,67 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>53</v>
       </c>

</xml_diff>

<commit_message>
Some changes on product editor...
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\Entwicklung\WildShop\WNodeJS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B18E427C-4338-41BD-8619-EC25CCE86BD9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2325F57-8415-4C3B-8F16-3C66AC71D7E4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315" activeTab="1" xr2:uid="{659A3680-8E12-4613-AC7A-D48333959E04}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="74">
   <si>
     <t>TODO</t>
   </si>
@@ -246,6 +246,9 @@
   </si>
   <si>
     <t>Order anhand orderID suchen können</t>
+  </si>
+  <si>
+    <t>Vorbestellungen verschieben, wenn Amount geändert wird</t>
   </si>
 </sst>
 </file>
@@ -990,10 +993,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B04E74DD-7DA5-47AC-8294-8183086F3F5E}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1019,8 +1022,8 @@
       <c r="A2" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>9</v>
+      <c r="B2" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -1123,6 +1126,14 @@
       </c>
       <c r="C11" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Products can be deleted, updated and added now. Bugfixes in adding- and updating-process
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\Entwicklung\WildShop\WNodeJS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Jonas\Programmierung\Ionic\WildShop\WNodeJS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2325F57-8415-4C3B-8F16-3C66AC71D7E4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE86C184-4DC0-43C1-BA03-F91D54F1C47C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315" activeTab="1" xr2:uid="{659A3680-8E12-4613-AC7A-D48333959E04}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12312" activeTab="1" xr2:uid="{659A3680-8E12-4613-AC7A-D48333959E04}"/>
   </bookViews>
   <sheets>
     <sheet name="TODO" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="75">
   <si>
     <t>TODO</t>
   </si>
@@ -249,6 +249,9 @@
   </si>
   <si>
     <t>Vorbestellungen verschieben, wenn Amount geändert wird</t>
+  </si>
+  <si>
+    <t>Überhaupt sinnvoll?</t>
   </si>
 </sst>
 </file>
@@ -724,14 +727,14 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="69.140625" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="69.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -745,7 +748,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -756,7 +759,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -767,7 +770,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -778,7 +781,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -789,7 +792,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -803,7 +806,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -814,7 +817,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -825,7 +828,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -836,7 +839,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -847,7 +850,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -858,7 +861,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -866,7 +869,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -877,7 +880,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -888,7 +891,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -899,7 +902,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -910,7 +913,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -918,7 +921,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -926,7 +929,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>28</v>
       </c>
@@ -937,7 +940,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -945,7 +948,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -953,7 +956,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -961,7 +964,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>56</v>
       </c>
@@ -969,7 +972,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>61</v>
       </c>
@@ -977,7 +980,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>63</v>
       </c>
@@ -996,15 +999,15 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.85546875" customWidth="1"/>
+    <col min="1" max="1" width="36.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1018,7 +1021,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>64</v>
       </c>
@@ -1029,7 +1032,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1040,7 +1043,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>65</v>
       </c>
@@ -1050,30 +1053,33 @@
       <c r="C4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>66</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
+      <c r="B5" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>67</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>9</v>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>68</v>
       </c>
@@ -1084,7 +1090,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>69</v>
       </c>
@@ -1095,7 +1101,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>70</v>
       </c>
@@ -1106,7 +1112,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>71</v>
       </c>
@@ -1117,7 +1123,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>72</v>
       </c>
@@ -1128,7 +1134,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>73</v>
       </c>
@@ -1149,14 +1155,14 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="82.85546875" customWidth="1"/>
-    <col min="2" max="2" width="44.140625" customWidth="1"/>
-    <col min="3" max="3" width="41.7109375" customWidth="1"/>
+    <col min="1" max="1" width="82.88671875" customWidth="1"/>
+    <col min="2" max="2" width="44.109375" customWidth="1"/>
+    <col min="3" max="3" width="41.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>33</v>
       </c>
@@ -1167,7 +1173,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -1175,7 +1181,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -1183,7 +1189,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -1191,7 +1197,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -1199,7 +1205,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -1207,7 +1213,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -1215,7 +1221,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -1223,67 +1229,67 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>53</v>
       </c>

</xml_diff>

<commit_message>
Implemented searching in products and in orders (tested partwise).
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Jonas\Programmierung\Ionic\WildShop\WNodeJS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE86C184-4DC0-43C1-BA03-F91D54F1C47C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECB415A9-1C70-41CE-8D32-B7560E2170B7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12312" activeTab="1" xr2:uid="{659A3680-8E12-4613-AC7A-D48333959E04}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="78">
   <si>
     <t>TODO</t>
   </si>
@@ -252,6 +252,15 @@
   </si>
   <si>
     <t>Überhaupt sinnvoll?</t>
+  </si>
+  <si>
+    <t>Bestellungen suchen</t>
+  </si>
+  <si>
+    <t>Produkte suchen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doku schreiben </t>
   </si>
 </sst>
 </file>
@@ -996,10 +1005,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B04E74DD-7DA5-47AC-8294-8183086F3F5E}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B15" activeCellId="1" sqref="B12 B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1127,8 +1136,8 @@
       <c r="A11" t="s">
         <v>72</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>9</v>
+      <c r="B11" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
@@ -1139,6 +1148,30 @@
         <v>73</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Verficiation-process implemented, but not tested.
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Jonas\Programmierung\Ionic\WildShop\WNodeJS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECB415A9-1C70-41CE-8D32-B7560E2170B7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{785CB481-EC69-423C-B786-BCAD20D3FC84}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12312" activeTab="1" xr2:uid="{659A3680-8E12-4613-AC7A-D48333959E04}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12312" xr2:uid="{659A3680-8E12-4613-AC7A-D48333959E04}"/>
   </bookViews>
   <sheets>
     <sheet name="TODO" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="80">
   <si>
     <t>TODO</t>
   </si>
@@ -261,6 +261,12 @@
   </si>
   <si>
     <t xml:space="preserve">Doku schreiben </t>
+  </si>
+  <si>
+    <t>Strings (z.B. in MailController) in Datei auslagern</t>
+  </si>
+  <si>
+    <t>Strings in MailController in Datei auslagern</t>
   </si>
 </sst>
 </file>
@@ -730,10 +736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D9FE81-AB7B-4C47-91AF-D3A27946C115}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -997,6 +1003,14 @@
         <v>9</v>
       </c>
     </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>79</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -1005,10 +1019,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B04E74DD-7DA5-47AC-8294-8183086F3F5E}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" activeCellId="1" sqref="B12 B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1172,6 +1186,14 @@
         <v>77</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Improved order-moving, still not tested yet.
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Jonas\Programmierung\Ionic\WildShop\WNodeJS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{785CB481-EC69-423C-B786-BCAD20D3FC84}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD288D00-0C20-437E-8834-E989679CD650}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12312" xr2:uid="{659A3680-8E12-4613-AC7A-D48333959E04}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12312" activeTab="1" xr2:uid="{659A3680-8E12-4613-AC7A-D48333959E04}"/>
   </bookViews>
   <sheets>
     <sheet name="TODO" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="84">
   <si>
     <t>TODO</t>
   </si>
@@ -267,13 +267,25 @@
   </si>
   <si>
     <t>Strings in MailController in Datei auslagern</t>
+  </si>
+  <si>
+    <t>nicht getestet</t>
+  </si>
+  <si>
+    <t>Bilder hochladen</t>
+  </si>
+  <si>
+    <t>IP-Adressen loggen und deren Tätigkeit, am besten auch User-ID</t>
+  </si>
+  <si>
+    <t>IP-Adressen loggen und deren Tätigkeit, am besten auch User-Ids</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -318,8 +330,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -367,6 +386,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -381,7 +412,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
@@ -393,6 +424,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Schlecht" xfId="1" builtinId="27"/>
@@ -736,10 +770,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D9FE81-AB7B-4C47-91AF-D3A27946C115}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1011,6 +1045,14 @@
         <v>9</v>
       </c>
     </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>83</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -1019,23 +1061,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B04E74DD-7DA5-47AC-8294-8183086F3F5E}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.88671875" customWidth="1"/>
+    <col min="1" max="1" width="53" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
+      <c r="B1" s="12" t="s">
+        <v>9</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
@@ -1106,8 +1148,8 @@
       <c r="A7" t="s">
         <v>68</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>9</v>
+      <c r="B7" s="11" t="s">
+        <v>80</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
@@ -1117,8 +1159,8 @@
       <c r="A8" t="s">
         <v>69</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>9</v>
+      <c r="B8" s="11" t="s">
+        <v>80</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
@@ -1139,8 +1181,8 @@
       <c r="A10" t="s">
         <v>71</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>9</v>
+      <c r="B10" s="11" t="s">
+        <v>80</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
@@ -1161,8 +1203,8 @@
       <c r="A12" t="s">
         <v>73</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>9</v>
+      <c r="B12" s="11" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -1194,6 +1236,22 @@
         <v>78</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>82</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Logger logs activities of both pages, but in the wrong file -> in TODO is entered what to do
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Jonas\Programmierung\Ionic\WildShop\WNodeJS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD288D00-0C20-437E-8834-E989679CD650}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECA6C357-AA72-4244-9636-456BF4CA2317}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12312" activeTab="1" xr2:uid="{659A3680-8E12-4613-AC7A-D48333959E04}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="90">
   <si>
     <t>TODO</t>
   </si>
@@ -279,6 +279,24 @@
   </si>
   <si>
     <t>IP-Adressen loggen und deren Tätigkeit, am besten auch User-Ids</t>
+  </si>
+  <si>
+    <t>Bestätigung eines Admin-Accounts nur angemeldet</t>
+  </si>
+  <si>
+    <t>ProductPool anzeigen</t>
+  </si>
+  <si>
+    <t>Logger asynchron machen</t>
+  </si>
+  <si>
+    <t>zu späterem Zeitpunkt</t>
+  </si>
+  <si>
+    <t>Aus Logger Klasse machen -&gt; Instanziierung möglich</t>
+  </si>
+  <si>
+    <t>WICHTIG!!</t>
   </si>
 </sst>
 </file>
@@ -338,7 +356,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -398,6 +416,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -412,7 +436,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
@@ -427,6 +451,7 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Schlecht" xfId="1" builtinId="27"/>
@@ -1061,10 +1086,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B04E74DD-7DA5-47AC-8294-8183086F3F5E}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1112,8 +1137,8 @@
       <c r="A4" t="s">
         <v>65</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
+      <c r="B4" s="14" t="s">
+        <v>55</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
@@ -1239,7 +1264,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>81</v>
       </c>
@@ -1247,16 +1272,55 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>82</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>85</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>86</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>88</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Logger is using the right file now, some bug fixes and imporvements on product-page
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Jonas\Programmierung\Ionic\WildShop\WNodeJS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECA6C357-AA72-4244-9636-456BF4CA2317}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F3064B1-1DED-48DE-9AF8-AE15343C7C52}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12312" activeTab="1" xr2:uid="{659A3680-8E12-4613-AC7A-D48333959E04}"/>
   </bookViews>
@@ -1089,7 +1089,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1311,8 +1311,8 @@
       <c r="A22" t="s">
         <v>88</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>9</v>
+      <c r="B22" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="D22" t="s">
         <v>89</v>

</xml_diff>

<commit_message>
Added product-pool in cms. It's not perfectly running yet.
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Jonas\Programmierung\Ionic\WildShop\WNodeJS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F3064B1-1DED-48DE-9AF8-AE15343C7C52}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9260C15-D0AA-47ED-957D-FD099363B567}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12312" activeTab="1" xr2:uid="{659A3680-8E12-4613-AC7A-D48333959E04}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12312" activeTab="2" xr2:uid="{659A3680-8E12-4613-AC7A-D48333959E04}"/>
   </bookViews>
   <sheets>
     <sheet name="TODO" sheetId="1" r:id="rId1"/>
-    <sheet name="TODO CMS" sheetId="3" r:id="rId2"/>
-    <sheet name="Testfälle" sheetId="2" r:id="rId3"/>
+    <sheet name="Testfälle CMS" sheetId="4" r:id="rId2"/>
+    <sheet name="TODO CMS" sheetId="3" r:id="rId3"/>
+    <sheet name="Testfälle Shop" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="94">
   <si>
     <t>TODO</t>
   </si>
@@ -297,6 +298,18 @@
   </si>
   <si>
     <t>WICHTIG!!</t>
+  </si>
+  <si>
+    <t>Datenbank-User einschränken auf Mindestrechte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Datenbank-User beschränken auf Mindestrechte </t>
+  </si>
+  <si>
+    <t>E-Mail-Texte in Datenbank?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E-Mail-Text in Datenbank? </t>
   </si>
 </sst>
 </file>
@@ -795,10 +808,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D9FE81-AB7B-4C47-91AF-D3A27946C115}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1007,8 +1020,8 @@
       <c r="A19" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>9</v>
+      <c r="B19" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="D19" t="s">
         <v>54</v>
@@ -1075,6 +1088,22 @@
         <v>83</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>91</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>92</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1085,11 +1114,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DED5655-1A03-4429-8003-68282C2909C7}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B04E74DD-7DA5-47AC-8294-8183086F3F5E}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1292,8 +1333,8 @@
       <c r="A20" t="s">
         <v>85</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>9</v>
+      <c r="B20" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -1316,6 +1357,22 @@
       </c>
       <c r="D22" t="s">
         <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>90</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>93</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1324,7 +1381,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{398800B4-0215-4759-8FBC-1CB8B7366E83}">
   <dimension ref="A1:C21"/>
   <sheetViews>

</xml_diff>

<commit_message>
Server recognizes now if an product that should be added is already in the database, input-chechking implemented on client-side
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Jonas\Programmierung\Ionic\WildShop\WNodeJS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9260C15-D0AA-47ED-957D-FD099363B567}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{006404D9-5DB9-45F7-826C-0ABB55AC06EA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12312" activeTab="2" xr2:uid="{659A3680-8E12-4613-AC7A-D48333959E04}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="95">
   <si>
     <t>TODO</t>
   </si>
@@ -310,6 +310,9 @@
   </si>
   <si>
     <t xml:space="preserve">E-Mail-Text in Datenbank? </t>
+  </si>
+  <si>
+    <t>Eingabe testen</t>
   </si>
 </sst>
 </file>
@@ -1127,10 +1130,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B04E74DD-7DA5-47AC-8294-8183086F3F5E}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1317,8 +1320,8 @@
       <c r="A18" t="s">
         <v>82</v>
       </c>
-      <c r="B18" s="11" t="s">
-        <v>80</v>
+      <c r="B18" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -1372,6 +1375,14 @@
         <v>93</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>94</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Pushing to products and product-pool is now working, on delete will create an alert now
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Jonas\Programmierung\Ionic\WildShop\WNodeJS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{006404D9-5DB9-45F7-826C-0ABB55AC06EA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CE10782-389C-40CA-9583-731F122B20E2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12312" activeTab="2" xr2:uid="{659A3680-8E12-4613-AC7A-D48333959E04}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="96">
   <si>
     <t>TODO</t>
   </si>
@@ -313,6 +313,9 @@
   </si>
   <si>
     <t>Eingabe testen</t>
+  </si>
+  <si>
+    <t>console.logs entfernen</t>
   </si>
 </sst>
 </file>
@@ -811,10 +814,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D9FE81-AB7B-4C47-91AF-D3A27946C115}">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1090,8 +1093,8 @@
       <c r="A27" t="s">
         <v>83</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>9</v>
+      <c r="B27" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -1107,6 +1110,14 @@
         <v>92</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>95</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1130,10 +1141,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B04E74DD-7DA5-47AC-8294-8183086F3F5E}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1382,7 +1393,15 @@
       <c r="A25" t="s">
         <v>94</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>95</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>